<commit_message>
edited Task 5 excel
</commit_message>
<xml_diff>
--- a/assignment72/HeatForOMP/task_5_output/Task5.xlsx
+++ b/assignment72/HeatForOMP/task_5_output/Task5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hemra\Downloads\Programming_of_supercomputer\pos_21_group12\assignment72\HeatForOMP\task_5_output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{719C6B0D-A757-4E07-9FAF-02F0614FEE9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D1F8204-A3C0-4E44-9C50-AA2C568BC799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1231" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="151">
   <si>
     <t>Resolution</t>
   </si>
@@ -772,30 +772,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -828,6 +828,38 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>SpeedUp for </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>best MPI+OMP combination</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1997,6 +2029,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Configuration</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2062,6 +2149,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Speed Up</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2180,7 +2322,1560 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>MFlops</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> for </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>best MPI+OMP combination</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$A$90</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4500</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Tabelle1!$B$88:$L$89</c15:sqref>
+                  </c15:fullRef>
+                  <c15:levelRef>
+                    <c15:sqref>Tabelle1!$B$88:$L$88</c15:sqref>
+                  </c15:levelRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Tabelle1!$B$88:$L$88</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>MPI: 2x2 OMP: 48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MPI: 3x2 OMP: 32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MPI: 4x2 OMP: 24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MPI: 4x3 OMP: 16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MPI: 16x1 OMP: 12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>MPI: 3x8 OMP: 8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>MPI: 16x2 OMP: 6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>MPI: 16x3 OMP: 4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>MPI: 16x4 OMP: 3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>MPI: 8x12 OMP: 2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>MPI: 12x16 OMP: 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$B$90:$L$90</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>153135.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>163862.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>427144.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>259829.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>441300.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>477601.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>526074.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>480924.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>497462.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>570304.6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>505262.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-145B-463C-9FE7-5F5742DF6BA1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$A$91</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5500</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Tabelle1!$B$88:$L$89</c15:sqref>
+                  </c15:fullRef>
+                  <c15:levelRef>
+                    <c15:sqref>Tabelle1!$B$88:$L$88</c15:sqref>
+                  </c15:levelRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Tabelle1!$B$88:$L$88</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>MPI: 2x2 OMP: 48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MPI: 3x2 OMP: 32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MPI: 4x2 OMP: 24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MPI: 4x3 OMP: 16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MPI: 16x1 OMP: 12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>MPI: 3x8 OMP: 8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>MPI: 16x2 OMP: 6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>MPI: 16x3 OMP: 4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>MPI: 16x4 OMP: 3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>MPI: 8x12 OMP: 2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>MPI: 12x16 OMP: 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$B$91:$L$91</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>139940.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>137393.20000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>340683.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>243337.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>367335.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>354124.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>369613.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>358744.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>367016.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>377355.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>404759.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-145B-463C-9FE7-5F5742DF6BA1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$A$92</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>6500</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Tabelle1!$B$88:$L$89</c15:sqref>
+                  </c15:fullRef>
+                  <c15:levelRef>
+                    <c15:sqref>Tabelle1!$B$88:$L$88</c15:sqref>
+                  </c15:levelRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Tabelle1!$B$88:$L$88</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>MPI: 2x2 OMP: 48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MPI: 3x2 OMP: 32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MPI: 4x2 OMP: 24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MPI: 4x3 OMP: 16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MPI: 16x1 OMP: 12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>MPI: 3x8 OMP: 8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>MPI: 16x2 OMP: 6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>MPI: 16x3 OMP: 4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>MPI: 16x4 OMP: 3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>MPI: 8x12 OMP: 2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>MPI: 12x16 OMP: 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$B$92:$L$92</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>133283.79999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>131702.39999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>288648.09999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>217191.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>299614.90000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>286955.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>318971.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>317210</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>310578.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>312400.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>324750.40000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-145B-463C-9FE7-5F5742DF6BA1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$A$93</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>7500</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Tabelle1!$B$88:$L$89</c15:sqref>
+                  </c15:fullRef>
+                  <c15:levelRef>
+                    <c15:sqref>Tabelle1!$B$88:$L$88</c15:sqref>
+                  </c15:levelRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Tabelle1!$B$88:$L$88</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>MPI: 2x2 OMP: 48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MPI: 3x2 OMP: 32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MPI: 4x2 OMP: 24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MPI: 4x3 OMP: 16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MPI: 16x1 OMP: 12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>MPI: 3x8 OMP: 8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>MPI: 16x2 OMP: 6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>MPI: 16x3 OMP: 4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>MPI: 16x4 OMP: 3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>MPI: 8x12 OMP: 2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>MPI: 12x16 OMP: 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$B$93:$L$93</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>126717.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>111829</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>273847.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>201773.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>279095.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>267039.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>275957.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>284450.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>287578.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>274505.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>271730</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-145B-463C-9FE7-5F5742DF6BA1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$A$94</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>8500</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Tabelle1!$B$88:$L$89</c15:sqref>
+                  </c15:fullRef>
+                  <c15:levelRef>
+                    <c15:sqref>Tabelle1!$B$88:$L$88</c15:sqref>
+                  </c15:levelRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Tabelle1!$B$88:$L$88</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>MPI: 2x2 OMP: 48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MPI: 3x2 OMP: 32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MPI: 4x2 OMP: 24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MPI: 4x3 OMP: 16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MPI: 16x1 OMP: 12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>MPI: 3x8 OMP: 8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>MPI: 16x2 OMP: 6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>MPI: 16x3 OMP: 4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>MPI: 16x4 OMP: 3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>MPI: 8x12 OMP: 2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>MPI: 12x16 OMP: 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$B$94:$L$94</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>120815.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>117442.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>262829.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>198118.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>261322.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>253494.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>267154</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>270540.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>266668.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>266583.2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>273895.90000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-145B-463C-9FE7-5F5742DF6BA1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$A$95</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>9500</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Tabelle1!$B$88:$L$89</c15:sqref>
+                  </c15:fullRef>
+                  <c15:levelRef>
+                    <c15:sqref>Tabelle1!$B$88:$L$88</c15:sqref>
+                  </c15:levelRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Tabelle1!$B$88:$L$88</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>MPI: 2x2 OMP: 48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MPI: 3x2 OMP: 32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MPI: 4x2 OMP: 24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MPI: 4x3 OMP: 16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MPI: 16x1 OMP: 12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>MPI: 3x8 OMP: 8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>MPI: 16x2 OMP: 6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>MPI: 16x3 OMP: 4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>MPI: 16x4 OMP: 3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>MPI: 8x12 OMP: 2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>MPI: 12x16 OMP: 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$B$95:$L$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>120360.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>119275.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256601</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>193773.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>255546.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>255867.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>261887.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>259131.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>263493</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>257794.3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>255000.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-145B-463C-9FE7-5F5742DF6BA1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$A$96</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>10500</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Tabelle1!$B$88:$L$89</c15:sqref>
+                  </c15:fullRef>
+                  <c15:levelRef>
+                    <c15:sqref>Tabelle1!$B$88:$L$88</c15:sqref>
+                  </c15:levelRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Tabelle1!$B$88:$L$88</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>MPI: 2x2 OMP: 48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MPI: 3x2 OMP: 32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MPI: 4x2 OMP: 24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MPI: 4x3 OMP: 16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MPI: 16x1 OMP: 12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>MPI: 3x8 OMP: 8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>MPI: 16x2 OMP: 6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>MPI: 16x3 OMP: 4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>MPI: 16x4 OMP: 3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>MPI: 8x12 OMP: 2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>MPI: 12x16 OMP: 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$B$96:$L$96</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>120200.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>117842.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>245167.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>188900.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>251597.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>246117.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>250551.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>252879.1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256412.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>253648</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>248135.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-145B-463C-9FE7-5F5742DF6BA1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$A$97</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>11500</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Tabelle1!$B$88:$L$89</c15:sqref>
+                  </c15:fullRef>
+                  <c15:levelRef>
+                    <c15:sqref>Tabelle1!$B$88:$L$88</c15:sqref>
+                  </c15:levelRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Tabelle1!$B$88:$L$88</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>MPI: 2x2 OMP: 48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MPI: 3x2 OMP: 32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MPI: 4x2 OMP: 24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MPI: 4x3 OMP: 16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MPI: 16x1 OMP: 12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>MPI: 3x8 OMP: 8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>MPI: 16x2 OMP: 6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>MPI: 16x3 OMP: 4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>MPI: 16x4 OMP: 3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>MPI: 8x12 OMP: 2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>MPI: 12x16 OMP: 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$B$97:$L$97</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>118453.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>117870.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>246883</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>185673.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>246476.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>242270.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>252798.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>249626.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>251445.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>246833.6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>252347.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-145B-463C-9FE7-5F5742DF6BA1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$A$98</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>12500</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Tabelle1!$B$88:$L$89</c15:sqref>
+                  </c15:fullRef>
+                  <c15:levelRef>
+                    <c15:sqref>Tabelle1!$B$88:$L$88</c15:sqref>
+                  </c15:levelRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Tabelle1!$B$88:$L$88</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>MPI: 2x2 OMP: 48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MPI: 3x2 OMP: 32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MPI: 4x2 OMP: 24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MPI: 4x3 OMP: 16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MPI: 16x1 OMP: 12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>MPI: 3x8 OMP: 8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>MPI: 16x2 OMP: 6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>MPI: 16x3 OMP: 4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>MPI: 16x4 OMP: 3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>MPI: 8x12 OMP: 2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>MPI: 12x16 OMP: 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$B$98:$L$98</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>118244.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>118678.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>245226.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>185994.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>226651.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>238032.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>248182</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>250529.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>248876.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>244999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>247575.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-145B-463C-9FE7-5F5742DF6BA1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="833459199"/>
+        <c:axId val="833457951"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="833459199"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Configuration</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="833457951"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="833457951"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>MFlops</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="833459199"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2723,20 +4418,523 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>866775</xdr:colOff>
-      <xdr:row>86</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>657225</xdr:colOff>
-      <xdr:row>120</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2756,6 +4954,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9AFD06C-DF47-4621-845F-9B6CD05E748A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3027,10 +5261,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AY84"/>
+  <dimension ref="A1:AY98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C85" sqref="C85"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L98" sqref="A88:L98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3071,66 +5305,66 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37" t="s">
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37" t="s">
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="37"/>
-      <c r="S1" s="37" t="s">
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="T1" s="37"/>
-      <c r="U1" s="37"/>
-      <c r="V1" s="37"/>
-      <c r="W1" s="37"/>
-      <c r="X1" s="37" t="s">
+      <c r="T1" s="40"/>
+      <c r="U1" s="40"/>
+      <c r="V1" s="40"/>
+      <c r="W1" s="40"/>
+      <c r="X1" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="Y1" s="37"/>
-      <c r="Z1" s="37"/>
-      <c r="AA1" s="37"/>
-      <c r="AB1" s="37"/>
-      <c r="AC1" s="37"/>
-      <c r="AD1" s="37" t="s">
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="40"/>
+      <c r="AA1" s="40"/>
+      <c r="AB1" s="40"/>
+      <c r="AC1" s="40"/>
+      <c r="AD1" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="AE1" s="37"/>
-      <c r="AF1" s="37"/>
-      <c r="AG1" s="37"/>
-      <c r="AH1" s="37"/>
-      <c r="AI1" s="37"/>
-      <c r="AJ1" s="37"/>
-      <c r="AK1" s="37"/>
-      <c r="AL1" s="37" t="s">
+      <c r="AE1" s="40"/>
+      <c r="AF1" s="40"/>
+      <c r="AG1" s="40"/>
+      <c r="AH1" s="40"/>
+      <c r="AI1" s="40"/>
+      <c r="AJ1" s="40"/>
+      <c r="AK1" s="40"/>
+      <c r="AL1" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="AM1" s="37"/>
-      <c r="AN1" s="37"/>
-      <c r="AO1" s="37"/>
-      <c r="AP1" s="37"/>
-      <c r="AQ1" s="37"/>
-      <c r="AR1" s="37"/>
-      <c r="AS1" s="37"/>
-      <c r="AT1" s="37"/>
-      <c r="AU1" s="37"/>
-      <c r="AV1" s="37"/>
-      <c r="AW1" s="37"/>
-      <c r="AX1" s="37"/>
-      <c r="AY1" s="37"/>
+      <c r="AM1" s="40"/>
+      <c r="AN1" s="40"/>
+      <c r="AO1" s="40"/>
+      <c r="AP1" s="40"/>
+      <c r="AQ1" s="40"/>
+      <c r="AR1" s="40"/>
+      <c r="AS1" s="40"/>
+      <c r="AT1" s="40"/>
+      <c r="AU1" s="40"/>
+      <c r="AV1" s="40"/>
+      <c r="AW1" s="40"/>
+      <c r="AX1" s="40"/>
+      <c r="AY1" s="40"/>
     </row>
     <row r="2" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -4695,66 +6929,66 @@
       <c r="E15" t="s">
         <v>4</v>
       </c>
-      <c r="F15" s="37" t="s">
+      <c r="F15" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="37" t="s">
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="40"/>
+      <c r="K15" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="L15" s="37"/>
-      <c r="M15" s="37"/>
-      <c r="N15" s="37"/>
-      <c r="O15" s="37" t="s">
+      <c r="L15" s="40"/>
+      <c r="M15" s="40"/>
+      <c r="N15" s="40"/>
+      <c r="O15" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="P15" s="37"/>
-      <c r="Q15" s="37"/>
-      <c r="R15" s="37"/>
-      <c r="S15" s="37" t="s">
+      <c r="P15" s="40"/>
+      <c r="Q15" s="40"/>
+      <c r="R15" s="40"/>
+      <c r="S15" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="T15" s="37"/>
-      <c r="U15" s="37"/>
-      <c r="V15" s="37"/>
-      <c r="W15" s="37"/>
-      <c r="X15" s="37" t="s">
+      <c r="T15" s="40"/>
+      <c r="U15" s="40"/>
+      <c r="V15" s="40"/>
+      <c r="W15" s="40"/>
+      <c r="X15" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="Y15" s="37"/>
-      <c r="Z15" s="37"/>
-      <c r="AA15" s="37"/>
-      <c r="AB15" s="37"/>
-      <c r="AC15" s="37"/>
-      <c r="AD15" s="37" t="s">
+      <c r="Y15" s="40"/>
+      <c r="Z15" s="40"/>
+      <c r="AA15" s="40"/>
+      <c r="AB15" s="40"/>
+      <c r="AC15" s="40"/>
+      <c r="AD15" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="AE15" s="37"/>
-      <c r="AF15" s="37"/>
-      <c r="AG15" s="37"/>
-      <c r="AH15" s="37"/>
-      <c r="AI15" s="37"/>
-      <c r="AJ15" s="37"/>
-      <c r="AK15" s="37"/>
-      <c r="AL15" s="37" t="s">
+      <c r="AE15" s="40"/>
+      <c r="AF15" s="40"/>
+      <c r="AG15" s="40"/>
+      <c r="AH15" s="40"/>
+      <c r="AI15" s="40"/>
+      <c r="AJ15" s="40"/>
+      <c r="AK15" s="40"/>
+      <c r="AL15" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="AM15" s="37"/>
-      <c r="AN15" s="37"/>
-      <c r="AO15" s="37"/>
-      <c r="AP15" s="37"/>
-      <c r="AQ15" s="37"/>
-      <c r="AR15" s="37"/>
-      <c r="AS15" s="37"/>
-      <c r="AT15" s="37"/>
-      <c r="AU15" s="37"/>
-      <c r="AV15" s="37"/>
-      <c r="AW15" s="37"/>
-      <c r="AX15" s="37"/>
-      <c r="AY15" s="37"/>
+      <c r="AM15" s="40"/>
+      <c r="AN15" s="40"/>
+      <c r="AO15" s="40"/>
+      <c r="AP15" s="40"/>
+      <c r="AQ15" s="40"/>
+      <c r="AR15" s="40"/>
+      <c r="AS15" s="40"/>
+      <c r="AT15" s="40"/>
+      <c r="AU15" s="40"/>
+      <c r="AV15" s="40"/>
+      <c r="AW15" s="40"/>
+      <c r="AX15" s="40"/>
+      <c r="AY15" s="40"/>
     </row>
     <row r="16" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -6850,66 +9084,66 @@
       <c r="E42" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F42" s="39" t="s">
+      <c r="F42" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="G42" s="35"/>
-      <c r="H42" s="35"/>
-      <c r="I42" s="35"/>
-      <c r="J42" s="35"/>
-      <c r="K42" s="35" t="s">
+      <c r="G42" s="41"/>
+      <c r="H42" s="41"/>
+      <c r="I42" s="41"/>
+      <c r="J42" s="41"/>
+      <c r="K42" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="L42" s="35"/>
-      <c r="M42" s="35"/>
-      <c r="N42" s="38"/>
-      <c r="O42" s="34" t="s">
+      <c r="L42" s="41"/>
+      <c r="M42" s="41"/>
+      <c r="N42" s="42"/>
+      <c r="O42" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="P42" s="35"/>
-      <c r="Q42" s="35"/>
-      <c r="R42" s="36"/>
-      <c r="S42" s="34" t="s">
+      <c r="P42" s="41"/>
+      <c r="Q42" s="41"/>
+      <c r="R42" s="44"/>
+      <c r="S42" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="T42" s="35"/>
-      <c r="U42" s="35"/>
-      <c r="V42" s="35"/>
-      <c r="W42" s="36"/>
-      <c r="X42" s="34" t="s">
+      <c r="T42" s="41"/>
+      <c r="U42" s="41"/>
+      <c r="V42" s="41"/>
+      <c r="W42" s="44"/>
+      <c r="X42" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="Y42" s="35"/>
-      <c r="Z42" s="35"/>
-      <c r="AA42" s="35"/>
-      <c r="AB42" s="35"/>
-      <c r="AC42" s="36"/>
-      <c r="AD42" s="34" t="s">
+      <c r="Y42" s="41"/>
+      <c r="Z42" s="41"/>
+      <c r="AA42" s="41"/>
+      <c r="AB42" s="41"/>
+      <c r="AC42" s="44"/>
+      <c r="AD42" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="AE42" s="35"/>
-      <c r="AF42" s="35"/>
-      <c r="AG42" s="35"/>
-      <c r="AH42" s="35"/>
-      <c r="AI42" s="35"/>
-      <c r="AJ42" s="35"/>
-      <c r="AK42" s="36"/>
-      <c r="AL42" s="34" t="s">
+      <c r="AE42" s="41"/>
+      <c r="AF42" s="41"/>
+      <c r="AG42" s="41"/>
+      <c r="AH42" s="41"/>
+      <c r="AI42" s="41"/>
+      <c r="AJ42" s="41"/>
+      <c r="AK42" s="44"/>
+      <c r="AL42" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="AM42" s="35"/>
-      <c r="AN42" s="35"/>
-      <c r="AO42" s="35"/>
-      <c r="AP42" s="35"/>
-      <c r="AQ42" s="35"/>
-      <c r="AR42" s="35"/>
-      <c r="AS42" s="35"/>
-      <c r="AT42" s="35"/>
-      <c r="AU42" s="35"/>
-      <c r="AV42" s="35"/>
-      <c r="AW42" s="35"/>
-      <c r="AX42" s="35"/>
-      <c r="AY42" s="36"/>
+      <c r="AM42" s="41"/>
+      <c r="AN42" s="41"/>
+      <c r="AO42" s="41"/>
+      <c r="AP42" s="41"/>
+      <c r="AQ42" s="41"/>
+      <c r="AR42" s="41"/>
+      <c r="AS42" s="41"/>
+      <c r="AT42" s="41"/>
+      <c r="AU42" s="41"/>
+      <c r="AV42" s="41"/>
+      <c r="AW42" s="41"/>
+      <c r="AX42" s="41"/>
+      <c r="AY42" s="44"/>
     </row>
     <row r="43" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -8885,66 +11119,66 @@
       <c r="E58" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F58" s="34" t="s">
+      <c r="F58" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="G58" s="35"/>
-      <c r="H58" s="35"/>
-      <c r="I58" s="35"/>
-      <c r="J58" s="36"/>
-      <c r="K58" s="34" t="s">
+      <c r="G58" s="41"/>
+      <c r="H58" s="41"/>
+      <c r="I58" s="41"/>
+      <c r="J58" s="44"/>
+      <c r="K58" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="L58" s="35"/>
-      <c r="M58" s="35"/>
-      <c r="N58" s="36"/>
-      <c r="O58" s="34" t="s">
+      <c r="L58" s="41"/>
+      <c r="M58" s="41"/>
+      <c r="N58" s="44"/>
+      <c r="O58" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="P58" s="35"/>
-      <c r="Q58" s="35"/>
-      <c r="R58" s="36"/>
-      <c r="S58" s="34" t="s">
+      <c r="P58" s="41"/>
+      <c r="Q58" s="41"/>
+      <c r="R58" s="44"/>
+      <c r="S58" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="T58" s="35"/>
-      <c r="U58" s="35"/>
-      <c r="V58" s="35"/>
-      <c r="W58" s="36"/>
-      <c r="X58" s="34" t="s">
+      <c r="T58" s="41"/>
+      <c r="U58" s="41"/>
+      <c r="V58" s="41"/>
+      <c r="W58" s="44"/>
+      <c r="X58" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="Y58" s="35"/>
-      <c r="Z58" s="35"/>
-      <c r="AA58" s="35"/>
-      <c r="AB58" s="35"/>
-      <c r="AC58" s="36"/>
-      <c r="AD58" s="34" t="s">
+      <c r="Y58" s="41"/>
+      <c r="Z58" s="41"/>
+      <c r="AA58" s="41"/>
+      <c r="AB58" s="41"/>
+      <c r="AC58" s="44"/>
+      <c r="AD58" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="AE58" s="35"/>
-      <c r="AF58" s="35"/>
-      <c r="AG58" s="35"/>
-      <c r="AH58" s="35"/>
-      <c r="AI58" s="35"/>
-      <c r="AJ58" s="35"/>
-      <c r="AK58" s="36"/>
-      <c r="AL58" s="34" t="s">
+      <c r="AE58" s="41"/>
+      <c r="AF58" s="41"/>
+      <c r="AG58" s="41"/>
+      <c r="AH58" s="41"/>
+      <c r="AI58" s="41"/>
+      <c r="AJ58" s="41"/>
+      <c r="AK58" s="44"/>
+      <c r="AL58" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="AM58" s="35"/>
-      <c r="AN58" s="35"/>
-      <c r="AO58" s="35"/>
-      <c r="AP58" s="35"/>
-      <c r="AQ58" s="35"/>
-      <c r="AR58" s="35"/>
-      <c r="AS58" s="35"/>
-      <c r="AT58" s="35"/>
-      <c r="AU58" s="35"/>
-      <c r="AV58" s="35"/>
-      <c r="AW58" s="35"/>
-      <c r="AX58" s="35"/>
-      <c r="AY58" s="36"/>
+      <c r="AM58" s="41"/>
+      <c r="AN58" s="41"/>
+      <c r="AO58" s="41"/>
+      <c r="AP58" s="41"/>
+      <c r="AQ58" s="41"/>
+      <c r="AR58" s="41"/>
+      <c r="AS58" s="41"/>
+      <c r="AT58" s="41"/>
+      <c r="AU58" s="41"/>
+      <c r="AV58" s="41"/>
+      <c r="AW58" s="41"/>
+      <c r="AX58" s="41"/>
+      <c r="AY58" s="44"/>
     </row>
     <row r="59" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
@@ -9117,7 +11351,7 @@
       <c r="E60" s="15">
         <v>259829.8</v>
       </c>
-      <c r="F60" s="40">
+      <c r="F60" s="34">
         <v>441300.9</v>
       </c>
       <c r="G60" s="12">
@@ -9138,13 +11372,13 @@
       <c r="L60" s="12">
         <v>384307.3</v>
       </c>
-      <c r="M60" s="42">
+      <c r="M60" s="36">
         <v>477601.8</v>
       </c>
       <c r="N60" s="13">
         <v>3561.1</v>
       </c>
-      <c r="O60" s="40">
+      <c r="O60" s="34">
         <v>526074.1</v>
       </c>
       <c r="P60" s="12">
@@ -9156,7 +11390,7 @@
       <c r="R60" s="13">
         <v>309932</v>
       </c>
-      <c r="S60" s="40">
+      <c r="S60" s="34">
         <v>480924.2</v>
       </c>
       <c r="T60" s="12">
@@ -9171,7 +11405,7 @@
       <c r="W60" s="13">
         <v>349094.40000000002</v>
       </c>
-      <c r="X60" s="40">
+      <c r="X60" s="34">
         <v>497462.7</v>
       </c>
       <c r="Y60" s="12">
@@ -9210,7 +11444,7 @@
       <c r="AJ60" s="12">
         <v>531886.4</v>
       </c>
-      <c r="AK60" s="44">
+      <c r="AK60" s="38">
         <v>570304.6</v>
       </c>
       <c r="AL60" s="11">
@@ -9219,7 +11453,7 @@
       <c r="AM60" s="12">
         <v>188447.5</v>
       </c>
-      <c r="AN60" s="42">
+      <c r="AN60" s="36">
         <v>505262.7</v>
       </c>
       <c r="AO60" s="12">
@@ -9272,7 +11506,7 @@
       <c r="E61" s="15">
         <v>243337.1</v>
       </c>
-      <c r="F61" s="40">
+      <c r="F61" s="34">
         <v>367335.5</v>
       </c>
       <c r="G61" s="12">
@@ -9293,13 +11527,13 @@
       <c r="L61" s="12">
         <v>365431.2</v>
       </c>
-      <c r="M61" s="42">
+      <c r="M61" s="36">
         <v>354124.4</v>
       </c>
       <c r="N61" s="13">
         <v>324299.90000000002</v>
       </c>
-      <c r="O61" s="40">
+      <c r="O61" s="34">
         <v>369613.3</v>
       </c>
       <c r="P61" s="12">
@@ -9311,7 +11545,7 @@
       <c r="R61" s="13">
         <v>356455.2</v>
       </c>
-      <c r="S61" s="40">
+      <c r="S61" s="34">
         <v>358744.5</v>
       </c>
       <c r="T61" s="12">
@@ -9326,7 +11560,7 @@
       <c r="W61" s="13">
         <v>361998</v>
       </c>
-      <c r="X61" s="40">
+      <c r="X61" s="34">
         <v>367016.8</v>
       </c>
       <c r="Y61" s="12">
@@ -9365,7 +11599,7 @@
       <c r="AJ61" s="12">
         <v>385136.4</v>
       </c>
-      <c r="AK61" s="44">
+      <c r="AK61" s="38">
         <v>377355.5</v>
       </c>
       <c r="AL61" s="11">
@@ -9374,7 +11608,7 @@
       <c r="AM61" s="12">
         <v>380304.4</v>
       </c>
-      <c r="AN61" s="42">
+      <c r="AN61" s="36">
         <v>404759.7</v>
       </c>
       <c r="AO61" s="12">
@@ -9427,7 +11661,7 @@
       <c r="E62" s="15">
         <v>217191.1</v>
       </c>
-      <c r="F62" s="40">
+      <c r="F62" s="34">
         <v>299614.90000000002</v>
       </c>
       <c r="G62" s="12">
@@ -9448,13 +11682,13 @@
       <c r="L62" s="12">
         <v>300697</v>
       </c>
-      <c r="M62" s="42">
+      <c r="M62" s="36">
         <v>286955.5</v>
       </c>
       <c r="N62" s="13">
         <v>293094.90000000002</v>
       </c>
-      <c r="O62" s="40">
+      <c r="O62" s="34">
         <v>318971.8</v>
       </c>
       <c r="P62" s="12">
@@ -9466,7 +11700,7 @@
       <c r="R62" s="13">
         <v>286329.5</v>
       </c>
-      <c r="S62" s="40">
+      <c r="S62" s="34">
         <v>317210</v>
       </c>
       <c r="T62" s="12">
@@ -9481,7 +11715,7 @@
       <c r="W62" s="13">
         <v>312514.90000000002</v>
       </c>
-      <c r="X62" s="40">
+      <c r="X62" s="34">
         <v>310578.3</v>
       </c>
       <c r="Y62" s="12">
@@ -9520,7 +11754,7 @@
       <c r="AJ62" s="12">
         <v>312467.7</v>
       </c>
-      <c r="AK62" s="44">
+      <c r="AK62" s="38">
         <v>312400.8</v>
       </c>
       <c r="AL62" s="11">
@@ -9529,7 +11763,7 @@
       <c r="AM62" s="12">
         <v>295528.3</v>
       </c>
-      <c r="AN62" s="42">
+      <c r="AN62" s="36">
         <v>324750.40000000002</v>
       </c>
       <c r="AO62" s="12">
@@ -9582,7 +11816,7 @@
       <c r="E63" s="15">
         <v>201773.6</v>
       </c>
-      <c r="F63" s="40">
+      <c r="F63" s="34">
         <v>279095.7</v>
       </c>
       <c r="G63" s="12">
@@ -9603,13 +11837,13 @@
       <c r="L63" s="12">
         <v>276199.5</v>
       </c>
-      <c r="M63" s="42">
+      <c r="M63" s="36">
         <v>267039.7</v>
       </c>
       <c r="N63" s="13">
         <v>265249.09999999998</v>
       </c>
-      <c r="O63" s="40">
+      <c r="O63" s="34">
         <v>275957.2</v>
       </c>
       <c r="P63" s="12">
@@ -9621,7 +11855,7 @@
       <c r="R63" s="13">
         <v>274448.40000000002</v>
       </c>
-      <c r="S63" s="40">
+      <c r="S63" s="34">
         <v>284450.8</v>
       </c>
       <c r="T63" s="12">
@@ -9636,7 +11870,7 @@
       <c r="W63" s="13">
         <v>277592.2</v>
       </c>
-      <c r="X63" s="40">
+      <c r="X63" s="34">
         <v>287578.7</v>
       </c>
       <c r="Y63" s="12">
@@ -9675,7 +11909,7 @@
       <c r="AJ63" s="12">
         <v>283100.2</v>
       </c>
-      <c r="AK63" s="44">
+      <c r="AK63" s="38">
         <v>274505.5</v>
       </c>
       <c r="AL63" s="11">
@@ -9684,7 +11918,7 @@
       <c r="AM63" s="12">
         <v>256674.4</v>
       </c>
-      <c r="AN63" s="42">
+      <c r="AN63" s="36">
         <v>271730</v>
       </c>
       <c r="AO63" s="12">
@@ -9737,7 +11971,7 @@
       <c r="E64" s="15">
         <v>198118.9</v>
       </c>
-      <c r="F64" s="40">
+      <c r="F64" s="34">
         <v>261322.1</v>
       </c>
       <c r="G64" s="12">
@@ -9758,13 +11992,13 @@
       <c r="L64" s="12">
         <v>259739.8</v>
       </c>
-      <c r="M64" s="42">
+      <c r="M64" s="36">
         <v>253494.7</v>
       </c>
       <c r="N64" s="13">
         <v>260992.6</v>
       </c>
-      <c r="O64" s="40">
+      <c r="O64" s="34">
         <v>267154</v>
       </c>
       <c r="P64" s="12">
@@ -9776,7 +12010,7 @@
       <c r="R64" s="13">
         <v>264900.40000000002</v>
       </c>
-      <c r="S64" s="40">
+      <c r="S64" s="34">
         <v>270540.7</v>
       </c>
       <c r="T64" s="12">
@@ -9791,7 +12025,7 @@
       <c r="W64" s="13">
         <v>264887.09999999998</v>
       </c>
-      <c r="X64" s="40">
+      <c r="X64" s="34">
         <v>266668.7</v>
       </c>
       <c r="Y64" s="12">
@@ -9830,7 +12064,7 @@
       <c r="AJ64" s="12">
         <v>271952.40000000002</v>
       </c>
-      <c r="AK64" s="44">
+      <c r="AK64" s="38">
         <v>266583.2</v>
       </c>
       <c r="AL64" s="11">
@@ -9839,7 +12073,7 @@
       <c r="AM64" s="12">
         <v>262557.7</v>
       </c>
-      <c r="AN64" s="42">
+      <c r="AN64" s="36">
         <v>273895.90000000002</v>
       </c>
       <c r="AO64" s="12">
@@ -9892,7 +12126,7 @@
       <c r="E65" s="15">
         <v>193773.9</v>
       </c>
-      <c r="F65" s="40">
+      <c r="F65" s="34">
         <v>255546.8</v>
       </c>
       <c r="G65" s="12">
@@ -9913,13 +12147,13 @@
       <c r="L65" s="12">
         <v>255402.7</v>
       </c>
-      <c r="M65" s="42">
+      <c r="M65" s="36">
         <v>255867.5</v>
       </c>
       <c r="N65" s="13">
         <v>256194.1</v>
       </c>
-      <c r="O65" s="40">
+      <c r="O65" s="34">
         <v>261887.5</v>
       </c>
       <c r="P65" s="12">
@@ -9931,7 +12165,7 @@
       <c r="R65" s="13">
         <v>255330.1</v>
       </c>
-      <c r="S65" s="40">
+      <c r="S65" s="34">
         <v>259131.7</v>
       </c>
       <c r="T65" s="12">
@@ -9946,7 +12180,7 @@
       <c r="W65" s="13">
         <v>262311.40000000002</v>
       </c>
-      <c r="X65" s="40">
+      <c r="X65" s="34">
         <v>263493</v>
       </c>
       <c r="Y65" s="12">
@@ -9985,7 +12219,7 @@
       <c r="AJ65" s="12">
         <v>259536.6</v>
       </c>
-      <c r="AK65" s="44">
+      <c r="AK65" s="38">
         <v>257794.3</v>
       </c>
       <c r="AL65" s="11">
@@ -9994,7 +12228,7 @@
       <c r="AM65" s="12">
         <v>243660.9</v>
       </c>
-      <c r="AN65" s="42">
+      <c r="AN65" s="36">
         <v>255000.8</v>
       </c>
       <c r="AO65" s="12">
@@ -10047,7 +12281,7 @@
       <c r="E66" s="15">
         <v>188900.1</v>
       </c>
-      <c r="F66" s="40">
+      <c r="F66" s="34">
         <v>251597.6</v>
       </c>
       <c r="G66" s="12">
@@ -10068,13 +12302,13 @@
       <c r="L66" s="12">
         <v>246105.7</v>
       </c>
-      <c r="M66" s="42">
+      <c r="M66" s="36">
         <v>246117.8</v>
       </c>
       <c r="N66" s="13">
         <v>247402.6</v>
       </c>
-      <c r="O66" s="40">
+      <c r="O66" s="34">
         <v>250551.8</v>
       </c>
       <c r="P66" s="12">
@@ -10086,7 +12320,7 @@
       <c r="R66" s="13">
         <v>248602.5</v>
       </c>
-      <c r="S66" s="40">
+      <c r="S66" s="34">
         <v>252879.1</v>
       </c>
       <c r="T66" s="12">
@@ -10101,7 +12335,7 @@
       <c r="W66" s="13">
         <v>254963.6</v>
       </c>
-      <c r="X66" s="40">
+      <c r="X66" s="34">
         <v>256412.7</v>
       </c>
       <c r="Y66" s="12">
@@ -10140,7 +12374,7 @@
       <c r="AJ66" s="12">
         <v>250845</v>
       </c>
-      <c r="AK66" s="44">
+      <c r="AK66" s="38">
         <v>253648</v>
       </c>
       <c r="AL66" s="11">
@@ -10149,7 +12383,7 @@
       <c r="AM66" s="12">
         <v>242620.2</v>
       </c>
-      <c r="AN66" s="42">
+      <c r="AN66" s="36">
         <v>248135.6</v>
       </c>
       <c r="AO66" s="12">
@@ -10202,7 +12436,7 @@
       <c r="E67" s="15">
         <v>185673.4</v>
       </c>
-      <c r="F67" s="40">
+      <c r="F67" s="34">
         <v>246476.3</v>
       </c>
       <c r="G67" s="12">
@@ -10223,13 +12457,13 @@
       <c r="L67" s="12">
         <v>243637.6</v>
       </c>
-      <c r="M67" s="42">
+      <c r="M67" s="36">
         <v>242270.2</v>
       </c>
       <c r="N67" s="13">
         <v>247225.7</v>
       </c>
-      <c r="O67" s="40">
+      <c r="O67" s="34">
         <v>252798.9</v>
       </c>
       <c r="P67" s="12">
@@ -10241,7 +12475,7 @@
       <c r="R67" s="13">
         <v>248157.1</v>
       </c>
-      <c r="S67" s="40">
+      <c r="S67" s="34">
         <v>249626.4</v>
       </c>
       <c r="T67" s="12">
@@ -10256,7 +12490,7 @@
       <c r="W67" s="13">
         <v>252220</v>
       </c>
-      <c r="X67" s="40">
+      <c r="X67" s="34">
         <v>251445.8</v>
       </c>
       <c r="Y67" s="12">
@@ -10295,7 +12529,7 @@
       <c r="AJ67" s="12">
         <v>250077.4</v>
       </c>
-      <c r="AK67" s="44">
+      <c r="AK67" s="38">
         <v>246833.6</v>
       </c>
       <c r="AL67" s="11">
@@ -10304,7 +12538,7 @@
       <c r="AM67" s="12">
         <v>242089.7</v>
       </c>
-      <c r="AN67" s="42">
+      <c r="AN67" s="36">
         <v>252347.9</v>
       </c>
       <c r="AO67" s="12">
@@ -10357,7 +12591,7 @@
       <c r="E68" s="33">
         <v>185994.6</v>
       </c>
-      <c r="F68" s="41">
+      <c r="F68" s="35">
         <v>226651.1</v>
       </c>
       <c r="G68" s="31">
@@ -10378,13 +12612,13 @@
       <c r="L68" s="31">
         <v>240031</v>
       </c>
-      <c r="M68" s="43">
+      <c r="M68" s="37">
         <v>238032.7</v>
       </c>
       <c r="N68" s="32">
         <v>244853.8</v>
       </c>
-      <c r="O68" s="41">
+      <c r="O68" s="35">
         <v>248182</v>
       </c>
       <c r="P68" s="31">
@@ -10396,7 +12630,7 @@
       <c r="R68" s="32">
         <v>248941.6</v>
       </c>
-      <c r="S68" s="41">
+      <c r="S68" s="35">
         <v>250529.5</v>
       </c>
       <c r="T68" s="31">
@@ -10411,7 +12645,7 @@
       <c r="W68" s="32">
         <v>247050</v>
       </c>
-      <c r="X68" s="41">
+      <c r="X68" s="35">
         <v>248876.1</v>
       </c>
       <c r="Y68" s="31">
@@ -10450,7 +12684,7 @@
       <c r="AJ68" s="31">
         <v>245274.1</v>
       </c>
-      <c r="AK68" s="45">
+      <c r="AK68" s="39">
         <v>244999</v>
       </c>
       <c r="AL68" s="21">
@@ -10459,7 +12693,7 @@
       <c r="AM68" s="31">
         <v>242659.8</v>
       </c>
-      <c r="AN68" s="43">
+      <c r="AN68" s="37">
         <v>247575.3</v>
       </c>
       <c r="AO68" s="31">
@@ -11371,13 +13605,431 @@
       </c>
       <c r="M84" s="12"/>
     </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A88" s="23"/>
+      <c r="B88" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="C88" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="D88" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="E88" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="F88" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="G88" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="H88" s="29" t="s">
+        <v>146</v>
+      </c>
+      <c r="I88" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="J88" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="K88" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="L88" s="29" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A89" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B89" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="C89" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D89" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E89" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="F89" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="G89" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="H89" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="I89" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="J89" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="K89" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="L89" s="23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A90" s="23">
+        <v>4500</v>
+      </c>
+      <c r="B90" s="15">
+        <v>153135.9</v>
+      </c>
+      <c r="C90" s="15">
+        <v>163862.6</v>
+      </c>
+      <c r="D90" s="15">
+        <v>427144.6</v>
+      </c>
+      <c r="E90" s="15">
+        <v>259829.8</v>
+      </c>
+      <c r="F90" s="34">
+        <v>441300.9</v>
+      </c>
+      <c r="G90" s="36">
+        <v>477601.8</v>
+      </c>
+      <c r="H90" s="34">
+        <v>526074.1</v>
+      </c>
+      <c r="I90" s="34">
+        <v>480924.2</v>
+      </c>
+      <c r="J90" s="34">
+        <v>497462.7</v>
+      </c>
+      <c r="K90" s="38">
+        <v>570304.6</v>
+      </c>
+      <c r="L90" s="36">
+        <v>505262.7</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A91" s="23">
+        <v>5500</v>
+      </c>
+      <c r="B91" s="15">
+        <v>139940.1</v>
+      </c>
+      <c r="C91" s="15">
+        <v>137393.20000000001</v>
+      </c>
+      <c r="D91" s="15">
+        <v>340683.1</v>
+      </c>
+      <c r="E91" s="15">
+        <v>243337.1</v>
+      </c>
+      <c r="F91" s="34">
+        <v>367335.5</v>
+      </c>
+      <c r="G91" s="36">
+        <v>354124.4</v>
+      </c>
+      <c r="H91" s="34">
+        <v>369613.3</v>
+      </c>
+      <c r="I91" s="34">
+        <v>358744.5</v>
+      </c>
+      <c r="J91" s="34">
+        <v>367016.8</v>
+      </c>
+      <c r="K91" s="38">
+        <v>377355.5</v>
+      </c>
+      <c r="L91" s="36">
+        <v>404759.7</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A92" s="23">
+        <v>6500</v>
+      </c>
+      <c r="B92" s="15">
+        <v>133283.79999999999</v>
+      </c>
+      <c r="C92" s="15">
+        <v>131702.39999999999</v>
+      </c>
+      <c r="D92" s="15">
+        <v>288648.09999999998</v>
+      </c>
+      <c r="E92" s="15">
+        <v>217191.1</v>
+      </c>
+      <c r="F92" s="34">
+        <v>299614.90000000002</v>
+      </c>
+      <c r="G92" s="36">
+        <v>286955.5</v>
+      </c>
+      <c r="H92" s="34">
+        <v>318971.8</v>
+      </c>
+      <c r="I92" s="34">
+        <v>317210</v>
+      </c>
+      <c r="J92" s="34">
+        <v>310578.3</v>
+      </c>
+      <c r="K92" s="38">
+        <v>312400.8</v>
+      </c>
+      <c r="L92" s="36">
+        <v>324750.40000000002</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A93" s="23">
+        <v>7500</v>
+      </c>
+      <c r="B93" s="15">
+        <v>126717.8</v>
+      </c>
+      <c r="C93" s="15">
+        <v>111829</v>
+      </c>
+      <c r="D93" s="15">
+        <v>273847.7</v>
+      </c>
+      <c r="E93" s="15">
+        <v>201773.6</v>
+      </c>
+      <c r="F93" s="34">
+        <v>279095.7</v>
+      </c>
+      <c r="G93" s="36">
+        <v>267039.7</v>
+      </c>
+      <c r="H93" s="34">
+        <v>275957.2</v>
+      </c>
+      <c r="I93" s="34">
+        <v>284450.8</v>
+      </c>
+      <c r="J93" s="34">
+        <v>287578.7</v>
+      </c>
+      <c r="K93" s="38">
+        <v>274505.5</v>
+      </c>
+      <c r="L93" s="36">
+        <v>271730</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A94" s="23">
+        <v>8500</v>
+      </c>
+      <c r="B94" s="15">
+        <v>120815.3</v>
+      </c>
+      <c r="C94" s="15">
+        <v>117442.8</v>
+      </c>
+      <c r="D94" s="15">
+        <v>262829.3</v>
+      </c>
+      <c r="E94" s="15">
+        <v>198118.9</v>
+      </c>
+      <c r="F94" s="34">
+        <v>261322.1</v>
+      </c>
+      <c r="G94" s="36">
+        <v>253494.7</v>
+      </c>
+      <c r="H94" s="34">
+        <v>267154</v>
+      </c>
+      <c r="I94" s="34">
+        <v>270540.7</v>
+      </c>
+      <c r="J94" s="34">
+        <v>266668.7</v>
+      </c>
+      <c r="K94" s="38">
+        <v>266583.2</v>
+      </c>
+      <c r="L94" s="36">
+        <v>273895.90000000002</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A95" s="23">
+        <v>9500</v>
+      </c>
+      <c r="B95" s="15">
+        <v>120360.9</v>
+      </c>
+      <c r="C95" s="15">
+        <v>119275.7</v>
+      </c>
+      <c r="D95" s="15">
+        <v>256601</v>
+      </c>
+      <c r="E95" s="15">
+        <v>193773.9</v>
+      </c>
+      <c r="F95" s="34">
+        <v>255546.8</v>
+      </c>
+      <c r="G95" s="36">
+        <v>255867.5</v>
+      </c>
+      <c r="H95" s="34">
+        <v>261887.5</v>
+      </c>
+      <c r="I95" s="34">
+        <v>259131.7</v>
+      </c>
+      <c r="J95" s="34">
+        <v>263493</v>
+      </c>
+      <c r="K95" s="38">
+        <v>257794.3</v>
+      </c>
+      <c r="L95" s="36">
+        <v>255000.8</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A96" s="23">
+        <v>10500</v>
+      </c>
+      <c r="B96" s="15">
+        <v>120200.8</v>
+      </c>
+      <c r="C96" s="15">
+        <v>117842.4</v>
+      </c>
+      <c r="D96" s="15">
+        <v>245167.1</v>
+      </c>
+      <c r="E96" s="15">
+        <v>188900.1</v>
+      </c>
+      <c r="F96" s="34">
+        <v>251597.6</v>
+      </c>
+      <c r="G96" s="36">
+        <v>246117.8</v>
+      </c>
+      <c r="H96" s="34">
+        <v>250551.8</v>
+      </c>
+      <c r="I96" s="34">
+        <v>252879.1</v>
+      </c>
+      <c r="J96" s="34">
+        <v>256412.7</v>
+      </c>
+      <c r="K96" s="38">
+        <v>253648</v>
+      </c>
+      <c r="L96" s="36">
+        <v>248135.6</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A97" s="23">
+        <v>11500</v>
+      </c>
+      <c r="B97" s="15">
+        <v>118453.5</v>
+      </c>
+      <c r="C97" s="15">
+        <v>117870.6</v>
+      </c>
+      <c r="D97" s="15">
+        <v>246883</v>
+      </c>
+      <c r="E97" s="15">
+        <v>185673.4</v>
+      </c>
+      <c r="F97" s="34">
+        <v>246476.3</v>
+      </c>
+      <c r="G97" s="36">
+        <v>242270.2</v>
+      </c>
+      <c r="H97" s="34">
+        <v>252798.9</v>
+      </c>
+      <c r="I97" s="34">
+        <v>249626.4</v>
+      </c>
+      <c r="J97" s="34">
+        <v>251445.8</v>
+      </c>
+      <c r="K97" s="38">
+        <v>246833.6</v>
+      </c>
+      <c r="L97" s="36">
+        <v>252347.9</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="23">
+        <v>12500</v>
+      </c>
+      <c r="B98" s="33">
+        <v>118244.5</v>
+      </c>
+      <c r="C98" s="33">
+        <v>118678.7</v>
+      </c>
+      <c r="D98" s="33">
+        <v>245226.9</v>
+      </c>
+      <c r="E98" s="33">
+        <v>185994.6</v>
+      </c>
+      <c r="F98" s="35">
+        <v>226651.1</v>
+      </c>
+      <c r="G98" s="37">
+        <v>238032.7</v>
+      </c>
+      <c r="H98" s="35">
+        <v>248182</v>
+      </c>
+      <c r="I98" s="35">
+        <v>250529.5</v>
+      </c>
+      <c r="J98" s="35">
+        <v>248876.1</v>
+      </c>
+      <c r="K98" s="39">
+        <v>244999</v>
+      </c>
+      <c r="L98" s="37">
+        <v>247575.3</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="AD1:AK1"/>
-    <mergeCell ref="AL1:AY1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="O1:R1"/>
-    <mergeCell ref="S1:W1"/>
+    <mergeCell ref="AD58:AK58"/>
+    <mergeCell ref="AL58:AY58"/>
+    <mergeCell ref="F58:J58"/>
+    <mergeCell ref="K58:N58"/>
+    <mergeCell ref="O58:R58"/>
+    <mergeCell ref="S58:W58"/>
+    <mergeCell ref="X58:AC58"/>
     <mergeCell ref="F1:J1"/>
     <mergeCell ref="AD15:AK15"/>
     <mergeCell ref="AL15:AY15"/>
@@ -11394,13 +14046,11 @@
     <mergeCell ref="F15:J15"/>
     <mergeCell ref="F42:J42"/>
     <mergeCell ref="X1:AC1"/>
-    <mergeCell ref="AD58:AK58"/>
-    <mergeCell ref="AL58:AY58"/>
-    <mergeCell ref="F58:J58"/>
-    <mergeCell ref="K58:N58"/>
-    <mergeCell ref="O58:R58"/>
-    <mergeCell ref="S58:W58"/>
-    <mergeCell ref="X58:AC58"/>
+    <mergeCell ref="AD1:AK1"/>
+    <mergeCell ref="AL1:AY1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="S1:W1"/>
   </mergeCells>
   <conditionalFormatting sqref="F53:J53">
     <cfRule type="colorScale" priority="28">

</xml_diff>